<commit_message>
Data dimensions are adjusted
</commit_message>
<xml_diff>
--- a/data/SUTdata_long_format.xlsx
+++ b/data/SUTdata_long_format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="27">
   <si>
     <t>Country-product</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>GCF</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>EXP</t>
@@ -1951,7 +1948,7 @@
   <dimension ref="A1:G170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,10 +2266,10 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14">
         <v>1153.7755386102017</v>
@@ -2568,10 +2565,10 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G27">
         <v>763941.96055329905</v>
@@ -2867,10 +2864,10 @@
         <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G40">
         <v>2411.6562473537015</v>
@@ -3166,10 +3163,10 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G53">
         <v>234586.39470755</v>
@@ -3465,10 +3462,10 @@
         <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G66">
         <v>8180.5849926687661</v>
@@ -3764,10 +3761,10 @@
         <v>15</v>
       </c>
       <c r="E79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G79">
         <v>73312.236834776588</v>
@@ -4063,10 +4060,10 @@
         <v>16</v>
       </c>
       <c r="E92" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G92">
         <v>45.404385260888375</v>
@@ -4362,10 +4359,10 @@
         <v>17</v>
       </c>
       <c r="E105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G105">
         <v>118350.70903483592</v>
@@ -4379,10 +4376,10 @@
         <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D106" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E106" t="s">
         <v>8</v>
@@ -4402,10 +4399,10 @@
         <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E107" t="s">
         <v>8</v>
@@ -4425,10 +4422,10 @@
         <v>7</v>
       </c>
       <c r="C108" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E108" t="s">
         <v>8</v>
@@ -4448,10 +4445,10 @@
         <v>7</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E109" t="s">
         <v>8</v>
@@ -4471,10 +4468,10 @@
         <v>7</v>
       </c>
       <c r="C110" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D110" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E110" t="s">
         <v>10</v>
@@ -4494,10 +4491,10 @@
         <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D111" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E111" t="s">
         <v>10</v>
@@ -4517,10 +4514,10 @@
         <v>7</v>
       </c>
       <c r="C112" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D112" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E112" t="s">
         <v>10</v>
@@ -4540,10 +4537,10 @@
         <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D113" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E113" t="s">
         <v>10</v>
@@ -4563,10 +4560,10 @@
         <v>7</v>
       </c>
       <c r="C114" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E114" t="s">
         <v>8</v>
@@ -4586,10 +4583,10 @@
         <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D115" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E115" t="s">
         <v>8</v>
@@ -4609,10 +4606,10 @@
         <v>7</v>
       </c>
       <c r="C116" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D116" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E116" t="s">
         <v>10</v>
@@ -4632,10 +4629,10 @@
         <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D117" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E117" t="s">
         <v>10</v>
@@ -4655,16 +4652,16 @@
         <v>7</v>
       </c>
       <c r="C118" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118" t="s">
+        <v>22</v>
+      </c>
+      <c r="E118" t="s">
+        <v>21</v>
+      </c>
+      <c r="F118" t="s">
         <v>20</v>
-      </c>
-      <c r="D118" t="s">
-        <v>23</v>
-      </c>
-      <c r="E118" t="s">
-        <v>22</v>
-      </c>
-      <c r="F118" t="s">
-        <v>21</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4678,10 +4675,10 @@
         <v>7</v>
       </c>
       <c r="C119" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D119" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E119" t="s">
         <v>8</v>
@@ -4701,10 +4698,10 @@
         <v>7</v>
       </c>
       <c r="C120" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D120" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E120" t="s">
         <v>8</v>
@@ -4724,10 +4721,10 @@
         <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E121" t="s">
         <v>8</v>
@@ -4747,10 +4744,10 @@
         <v>7</v>
       </c>
       <c r="C122" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D122" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E122" t="s">
         <v>8</v>
@@ -4770,10 +4767,10 @@
         <v>7</v>
       </c>
       <c r="C123" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D123" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E123" t="s">
         <v>10</v>
@@ -4793,10 +4790,10 @@
         <v>7</v>
       </c>
       <c r="C124" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D124" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E124" t="s">
         <v>10</v>
@@ -4816,10 +4813,10 @@
         <v>7</v>
       </c>
       <c r="C125" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D125" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E125" t="s">
         <v>10</v>
@@ -4839,10 +4836,10 @@
         <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D126" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E126" t="s">
         <v>10</v>
@@ -4862,10 +4859,10 @@
         <v>7</v>
       </c>
       <c r="C127" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E127" t="s">
         <v>8</v>
@@ -4885,10 +4882,10 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D128" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E128" t="s">
         <v>8</v>
@@ -4908,10 +4905,10 @@
         <v>7</v>
       </c>
       <c r="C129" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D129" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E129" t="s">
         <v>10</v>
@@ -4931,10 +4928,10 @@
         <v>7</v>
       </c>
       <c r="C130" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D130" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E130" t="s">
         <v>10</v>
@@ -4954,16 +4951,16 @@
         <v>7</v>
       </c>
       <c r="C131" t="s">
+        <v>21</v>
+      </c>
+      <c r="D131" t="s">
+        <v>23</v>
+      </c>
+      <c r="E131" t="s">
+        <v>21</v>
+      </c>
+      <c r="F131" t="s">
         <v>20</v>
-      </c>
-      <c r="D131" t="s">
-        <v>24</v>
-      </c>
-      <c r="E131" t="s">
-        <v>22</v>
-      </c>
-      <c r="F131" t="s">
-        <v>21</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -4977,10 +4974,10 @@
         <v>7</v>
       </c>
       <c r="C132" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D132" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E132" t="s">
         <v>8</v>
@@ -5000,10 +4997,10 @@
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -5023,10 +5020,10 @@
         <v>7</v>
       </c>
       <c r="C134" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D134" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>
@@ -5046,10 +5043,10 @@
         <v>7</v>
       </c>
       <c r="C135" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D135" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E135" t="s">
         <v>8</v>
@@ -5069,10 +5066,10 @@
         <v>7</v>
       </c>
       <c r="C136" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D136" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E136" t="s">
         <v>10</v>
@@ -5092,10 +5089,10 @@
         <v>7</v>
       </c>
       <c r="C137" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D137" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E137" t="s">
         <v>10</v>
@@ -5115,10 +5112,10 @@
         <v>7</v>
       </c>
       <c r="C138" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D138" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E138" t="s">
         <v>10</v>
@@ -5138,10 +5135,10 @@
         <v>7</v>
       </c>
       <c r="C139" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D139" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E139" t="s">
         <v>10</v>
@@ -5161,10 +5158,10 @@
         <v>7</v>
       </c>
       <c r="C140" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D140" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E140" t="s">
         <v>8</v>
@@ -5184,10 +5181,10 @@
         <v>7</v>
       </c>
       <c r="C141" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D141" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E141" t="s">
         <v>8</v>
@@ -5207,10 +5204,10 @@
         <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D142" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E142" t="s">
         <v>10</v>
@@ -5230,10 +5227,10 @@
         <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D143" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E143" t="s">
         <v>10</v>
@@ -5253,16 +5250,16 @@
         <v>7</v>
       </c>
       <c r="C144" t="s">
+        <v>21</v>
+      </c>
+      <c r="D144" t="s">
+        <v>24</v>
+      </c>
+      <c r="E144" t="s">
+        <v>21</v>
+      </c>
+      <c r="F144" t="s">
         <v>20</v>
-      </c>
-      <c r="D144" t="s">
-        <v>25</v>
-      </c>
-      <c r="E144" t="s">
-        <v>22</v>
-      </c>
-      <c r="F144" t="s">
-        <v>21</v>
       </c>
       <c r="G144">
         <v>0</v>
@@ -5276,10 +5273,10 @@
         <v>7</v>
       </c>
       <c r="C145" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D145" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E145" t="s">
         <v>8</v>
@@ -5299,10 +5296,10 @@
         <v>7</v>
       </c>
       <c r="C146" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D146" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E146" t="s">
         <v>8</v>
@@ -5322,10 +5319,10 @@
         <v>7</v>
       </c>
       <c r="C147" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D147" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E147" t="s">
         <v>8</v>
@@ -5345,10 +5342,10 @@
         <v>7</v>
       </c>
       <c r="C148" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D148" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E148" t="s">
         <v>8</v>
@@ -5368,10 +5365,10 @@
         <v>7</v>
       </c>
       <c r="C149" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D149" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E149" t="s">
         <v>10</v>
@@ -5391,10 +5388,10 @@
         <v>7</v>
       </c>
       <c r="C150" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D150" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E150" t="s">
         <v>10</v>
@@ -5414,10 +5411,10 @@
         <v>7</v>
       </c>
       <c r="C151" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D151" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E151" t="s">
         <v>10</v>
@@ -5437,10 +5434,10 @@
         <v>7</v>
       </c>
       <c r="C152" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D152" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E152" t="s">
         <v>10</v>
@@ -5460,10 +5457,10 @@
         <v>7</v>
       </c>
       <c r="C153" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D153" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E153" t="s">
         <v>8</v>
@@ -5483,10 +5480,10 @@
         <v>7</v>
       </c>
       <c r="C154" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D154" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E154" t="s">
         <v>8</v>
@@ -5506,10 +5503,10 @@
         <v>7</v>
       </c>
       <c r="C155" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D155" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E155" t="s">
         <v>10</v>
@@ -5529,10 +5526,10 @@
         <v>7</v>
       </c>
       <c r="C156" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D156" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E156" t="s">
         <v>10</v>
@@ -5552,16 +5549,16 @@
         <v>7</v>
       </c>
       <c r="C157" t="s">
+        <v>21</v>
+      </c>
+      <c r="D157" t="s">
+        <v>25</v>
+      </c>
+      <c r="E157" t="s">
+        <v>21</v>
+      </c>
+      <c r="F157" t="s">
         <v>20</v>
-      </c>
-      <c r="D157" t="s">
-        <v>26</v>
-      </c>
-      <c r="E157" t="s">
-        <v>22</v>
-      </c>
-      <c r="F157" t="s">
-        <v>21</v>
       </c>
       <c r="G157">
         <v>0</v>
@@ -5575,10 +5572,10 @@
         <v>7</v>
       </c>
       <c r="C158" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D158" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E158" t="s">
         <v>8</v>
@@ -5598,10 +5595,10 @@
         <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E159" t="s">
         <v>8</v>
@@ -5621,10 +5618,10 @@
         <v>7</v>
       </c>
       <c r="C160" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D160" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E160" t="s">
         <v>8</v>
@@ -5644,10 +5641,10 @@
         <v>7</v>
       </c>
       <c r="C161" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E161" t="s">
         <v>8</v>
@@ -5667,10 +5664,10 @@
         <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D162" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E162" t="s">
         <v>10</v>
@@ -5690,10 +5687,10 @@
         <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D163" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E163" t="s">
         <v>10</v>
@@ -5713,10 +5710,10 @@
         <v>7</v>
       </c>
       <c r="C164" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D164" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E164" t="s">
         <v>10</v>
@@ -5736,10 +5733,10 @@
         <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D165" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E165" t="s">
         <v>10</v>
@@ -5759,10 +5756,10 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D166" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E166" t="s">
         <v>8</v>
@@ -5782,10 +5779,10 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D167" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E167" t="s">
         <v>8</v>
@@ -5805,10 +5802,10 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D168" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E168" t="s">
         <v>10</v>
@@ -5828,10 +5825,10 @@
         <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D169" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E169" t="s">
         <v>10</v>
@@ -5851,16 +5848,16 @@
         <v>7</v>
       </c>
       <c r="C170" t="s">
+        <v>21</v>
+      </c>
+      <c r="D170" t="s">
+        <v>26</v>
+      </c>
+      <c r="E170" t="s">
+        <v>21</v>
+      </c>
+      <c r="F170" t="s">
         <v>20</v>
-      </c>
-      <c r="D170" t="s">
-        <v>27</v>
-      </c>
-      <c r="E170" t="s">
-        <v>22</v>
-      </c>
-      <c r="F170" t="s">
-        <v>21</v>
       </c>
       <c r="G170">
         <v>0</v>

</xml_diff>